<commit_message>
Enable run for 250MT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget-CAP24_250MT.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget-CAP24_250MT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A4E57A-55AD-4E6A-AAC5-00E7A0952AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51289B23-608C-465D-A124-DDAFDDE12CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11175" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
   <si>
     <t>LimType</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>COM_CUMNET</t>
+  </si>
+  <si>
+    <t>UC_Sets: T_S:</t>
   </si>
 </sst>
 </file>
@@ -10032,8 +10035,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10058,19 +10061,19 @@
     </row>
     <row r="2" spans="1:12">
       <c r="B2" s="9" t="str">
-        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
-        <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <f>"UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
+        <v>UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" s="9" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="H4" t="str">
-        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
-        <v>~UC_T</v>
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","UC_T","")</f>
+        <v>UC_T</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10391,7 +10394,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>